<commit_message>
Fixed the beneficiary name column lengths to match the CCW Oracle schema.
Specifically, BENE_SRNM_NAME was 20 but should have been 24 and BENE_GVN_NAME was 20 but should have been 15.

CBBF-53
</commit_message>
<xml_diff>
--- a/bluebutton-data-model-rif/src/main/java/gov/hhs/cms/bluebutton/data/model/rif/rif-layout-and-fhir-mapping.xlsx
+++ b/bluebutton-data-model-rif/src/main/java/gov/hhs/cms/bluebutton/data/model/rif/rif-layout-and-fhir-mapping.xlsx
@@ -18875,7 +18875,7 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -19510,7 +19510,7 @@
         <v>29</v>
       </c>
       <c r="C19" s="17" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D19" s="17" t="s">
         <v>30</v>
@@ -19546,7 +19546,7 @@
         <v>29</v>
       </c>
       <c r="C20" s="17" t="n">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D20" s="17" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Bluebutton-885  renamed hicn history file to temp
</commit_message>
<xml_diff>
--- a/bluebutton-data-model-rif/src/main/java/gov/hhs/cms/bluebutton/data/model/rif/rif-layout-and-fhir-mapping.xlsx
+++ b/bluebutton-data-model-rif/src/main/java/gov/hhs/cms/bluebutton/data/model/rif/rif-layout-and-fhir-mapping.xlsx
@@ -3,18 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bit9prog\dev\gitrepo\bluebutton-data-model\bluebutton-data-model-rif\src\main\java\gov\hhs\cms\bluebutton\data\model\rif\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-72" yWindow="-72" windowWidth="38352" windowHeight="20940" tabRatio="487" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22152" windowHeight="7908" tabRatio="487" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
     <sheet name="Beneficiary" sheetId="2" r:id="rId2"/>
-    <sheet name="Beneficiary History New" sheetId="15" r:id="rId3"/>
+    <sheet name="Beneficiary History Temp" sheetId="15" r:id="rId3"/>
     <sheet name="Beneficiary History" sheetId="13" r:id="rId4"/>
     <sheet name="Medicare Beneficiary Id" sheetId="14" r:id="rId5"/>
     <sheet name="PDE" sheetId="3" r:id="rId6"/>
@@ -31,7 +26,8 @@
     <definedName name="CLM_ID" localSheetId="3">Carrier!#REF!</definedName>
     <definedName name="CLM_ID">Carrier!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -45447,8 +45443,8 @@
   <sheetPr published="0"/>
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update MbiHistory table's beneficiaryId
Changing the `beneficiaryId` in MbiHistory to a type varchar(15) for
consistency with other tables.
</commit_message>
<xml_diff>
--- a/bluebutton-data-model-rif/src/main/java/gov/hhs/cms/bluebutton/data/model/rif/rif-layout-and-fhir-mapping.xlsx
+++ b/bluebutton-data-model-rif/src/main/java/gov/hhs/cms/bluebutton/data/model/rif/rif-layout-and-fhir-mapping.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr autoCompressPictures="0"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bit9prog\dev\gitrepo\bluebutton-data-model\bluebutton-data-model-rif\src\main\java\gov\hhs\cms\bluebutton\data\model\rif\"/>
@@ -7909,7 +7909,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d\-mmm\-yyyy;@"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
@@ -40108,8 +40108,8 @@
   <sheetPr published="0"/>
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -40216,10 +40216,10 @@
         <v>1809</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>1735</v>
+        <v>1804</v>
       </c>
       <c r="C4" s="17">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D4" s="17" t="s">
         <v>1805</v>

</xml_diff>

<commit_message>
Updating rif layout with the correct type
BLUEBUTTON-1010
</commit_message>
<xml_diff>
--- a/bluebutton-data-model-rif/src/main/java/gov/hhs/cms/bluebutton/data/model/rif/rif-layout-and-fhir-mapping.xlsx
+++ b/bluebutton-data-model-rif/src/main/java/gov/hhs/cms/bluebutton/data/model/rif/rif-layout-and-fhir-mapping.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bit9prog\dev\gitrepo\bluebutton-data-model\bluebutton-data-model-rif\src\main\java\gov\hhs\cms\bluebutton\data\model\rif\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15648" windowHeight="3360" tabRatio="487" activeTab="2"/>
   </bookViews>
@@ -26,12 +31,11 @@
     <definedName name="CLM_ID">Carrier!#REF!</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:K25"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13707" uniqueCount="2624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13707" uniqueCount="2623">
   <si>
     <t>adjustmentReason</t>
   </si>
@@ -7900,9 +7904,6 @@
   </si>
   <si>
     <t>TIMESTAMP</t>
-  </si>
-  <si>
-    <t>NUMERIC</t>
   </si>
 </sst>
 </file>
@@ -9274,7 +9275,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -9309,7 +9310,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -39547,10 +39548,10 @@
         <v>1809</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>2623</v>
+        <v>1804</v>
       </c>
       <c r="C4" s="17">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D4" s="17" t="s">
         <v>1805</v>

</xml_diff>

<commit_message>
Revert "Updating rif layout with the correct type"
This reverts commit f0840697b84344f9927ce0a0b09013b0064cbfe0.
</commit_message>
<xml_diff>
--- a/bluebutton-data-model-rif/src/main/java/gov/hhs/cms/bluebutton/data/model/rif/rif-layout-and-fhir-mapping.xlsx
+++ b/bluebutton-data-model-rif/src/main/java/gov/hhs/cms/bluebutton/data/model/rif/rif-layout-and-fhir-mapping.xlsx
@@ -3,11 +3,6 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bit9prog\dev\gitrepo\bluebutton-data-model\bluebutton-data-model-rif\src\main\java\gov\hhs\cms\bluebutton\data\model\rif\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15648" windowHeight="3360" tabRatio="487" activeTab="2"/>
   </bookViews>
@@ -31,11 +26,12 @@
     <definedName name="CLM_ID">Carrier!#REF!</definedName>
   </definedNames>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:K25"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13707" uniqueCount="2623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13707" uniqueCount="2624">
   <si>
     <t>adjustmentReason</t>
   </si>
@@ -7904,6 +7900,9 @@
   </si>
   <si>
     <t>TIMESTAMP</t>
+  </si>
+  <si>
+    <t>NUMERIC</t>
   </si>
 </sst>
 </file>
@@ -9275,7 +9274,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -9310,7 +9309,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -39548,10 +39547,10 @@
         <v>1809</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>1804</v>
+        <v>2623</v>
       </c>
       <c r="C4" s="17">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D4" s="17" t="s">
         <v>1805</v>

</xml_diff>

<commit_message>
Changed the wrong field in the previous commit, this fixes it
BLUEBUTTON-1010
</commit_message>
<xml_diff>
--- a/bluebutton-data-model-rif/src/main/java/gov/hhs/cms/bluebutton/data/model/rif/rif-layout-and-fhir-mapping.xlsx
+++ b/bluebutton-data-model-rif/src/main/java/gov/hhs/cms/bluebutton/data/model/rif/rif-layout-and-fhir-mapping.xlsx
@@ -3,8 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bit9prog\dev\gitrepo\bluebutton-data-model\bluebutton-data-model-rif\src\main\java\gov\hhs\cms\bluebutton\data\model\rif\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15648" windowHeight="3360" tabRatio="487" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15648" windowHeight="3360" tabRatio="487" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -26,12 +31,11 @@
     <definedName name="CLM_ID">Carrier!#REF!</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:K25"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13707" uniqueCount="2624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13707" uniqueCount="2623">
   <si>
     <t>adjustmentReason</t>
   </si>
@@ -7900,9 +7904,6 @@
   </si>
   <si>
     <t>TIMESTAMP</t>
-  </si>
-  <si>
-    <t>NUMERIC</t>
   </si>
 </sst>
 </file>
@@ -9274,7 +9275,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -9309,7 +9310,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -39432,7 +39433,7 @@
   <sheetPr published="0"/>
   <dimension ref="A1:AMK21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -39547,10 +39548,10 @@
         <v>1809</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>2623</v>
+        <v>1804</v>
       </c>
       <c r="C4" s="17">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D4" s="17" t="s">
         <v>1805</v>
@@ -40107,8 +40108,8 @@
   <sheetPr published="0"/>
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -40215,10 +40216,10 @@
         <v>1809</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>1735</v>
+        <v>1804</v>
       </c>
       <c r="C4" s="17">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D4" s="17" t="s">
         <v>1805</v>

</xml_diff>

<commit_message>
Bluebutton-1076 - added data frequency to Beneficiary data
</commit_message>
<xml_diff>
--- a/bluebutton-data-model-rif/src/main/java/gov/hhs/cms/bluebutton/data/model/rif/rif-layout-and-fhir-mapping.xlsx
+++ b/bluebutton-data-model-rif/src/main/java/gov/hhs/cms/bluebutton/data/model/rif/rif-layout-and-fhir-mapping.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bit9prog\dev\gitrepo\bluebutton-data-model\bluebutton-data-model-rif\src\main\java\gov\hhs\cms\bluebutton\data\model\rif\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15648" windowHeight="3360" tabRatio="487" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22104" windowHeight="7836" tabRatio="487" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -31,11 +26,12 @@
     <definedName name="CLM_ID">Carrier!#REF!</definedName>
   </definedNames>
   <calcPr calcId="0"/>
+  <oleSize ref="A15:K29"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13707" uniqueCount="2623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13901" uniqueCount="2626">
   <si>
     <t>adjustmentReason</t>
   </si>
@@ -7904,12 +7900,21 @@
   </si>
   <si>
     <t>TIMESTAMP</t>
+  </si>
+  <si>
+    <t>Data Refresh Frequency</t>
+  </si>
+  <si>
+    <t>weekly</t>
+  </si>
+  <si>
+    <t>monthly</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d\-mmm\-yyyy;@"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
@@ -8676,7 +8681,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="175">
+  <cellXfs count="176">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -9088,6 +9093,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -14005,12 +14013,12 @@
       <c r="E98" s="82"/>
       <c r="F98" s="82"/>
       <c r="G98" s="82"/>
-      <c r="H98" s="174" t="s">
+      <c r="H98" s="175" t="s">
         <v>1225</v>
       </c>
-      <c r="I98" s="174"/>
-      <c r="J98" s="174"/>
-      <c r="K98" s="174"/>
+      <c r="I98" s="175"/>
+      <c r="J98" s="175"/>
+      <c r="K98" s="175"/>
       <c r="L98" s="93"/>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.3">
@@ -19901,12 +19909,12 @@
       <c r="E132" s="97"/>
       <c r="F132" s="82"/>
       <c r="G132" s="82"/>
-      <c r="H132" s="174" t="s">
+      <c r="H132" s="175" t="s">
         <v>1225</v>
       </c>
-      <c r="I132" s="174"/>
-      <c r="J132" s="174"/>
-      <c r="K132" s="174"/>
+      <c r="I132" s="175"/>
+      <c r="J132" s="175"/>
+      <c r="K132" s="175"/>
       <c r="L132" s="93"/>
     </row>
     <row r="133" spans="1:12" x14ac:dyDescent="0.3">
@@ -29382,12 +29390,12 @@
       <c r="E232" s="92"/>
       <c r="F232" s="82"/>
       <c r="G232" s="82"/>
-      <c r="H232" s="174" t="s">
+      <c r="H232" s="175" t="s">
         <v>1225</v>
       </c>
-      <c r="I232" s="174"/>
-      <c r="J232" s="174"/>
-      <c r="K232" s="174"/>
+      <c r="I232" s="175"/>
+      <c r="J232" s="175"/>
+      <c r="K232" s="175"/>
       <c r="L232" s="93"/>
     </row>
     <row r="233" spans="1:12" x14ac:dyDescent="0.3">
@@ -33567,10 +33575,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0"/>
-  <dimension ref="A1:AMK195"/>
+  <dimension ref="A1:AML195"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" topLeftCell="H25" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33580,33 +33588,34 @@
     <col min="6" max="6" width="13" style="6" customWidth="1"/>
     <col min="7" max="7" width="28.77734375" style="2" customWidth="1"/>
     <col min="8" max="8" width="33.88671875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="32" style="2" customWidth="1"/>
-    <col min="10" max="10" width="15.109375" style="6" customWidth="1"/>
-    <col min="11" max="11" width="8.5546875" style="6"/>
-    <col min="12" max="12" width="8.5546875" style="7"/>
-    <col min="13" max="13" width="8.5546875" style="8"/>
-    <col min="14" max="1025" width="8.5546875" style="2"/>
+    <col min="9" max="10" width="37.44140625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="15.109375" style="6" customWidth="1"/>
+    <col min="12" max="12" width="8.5546875" style="6"/>
+    <col min="13" max="13" width="8.5546875" style="7"/>
+    <col min="14" max="14" width="8.5546875" style="8"/>
+    <col min="15" max="1026" width="8.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="170" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="171" t="s">
         <v>1789</v>
       </c>
-      <c r="B1" s="170"/>
-      <c r="C1" s="170"/>
-      <c r="D1" s="170"/>
-      <c r="E1" s="170"/>
-      <c r="F1" s="170"/>
-      <c r="G1" s="170"/>
-      <c r="H1" s="170"/>
-      <c r="I1" s="170"/>
-      <c r="J1" s="171" t="s">
+      <c r="B1" s="171"/>
+      <c r="C1" s="171"/>
+      <c r="D1" s="171"/>
+      <c r="E1" s="171"/>
+      <c r="F1" s="171"/>
+      <c r="G1" s="171"/>
+      <c r="H1" s="171"/>
+      <c r="I1" s="171"/>
+      <c r="J1" s="170"/>
+      <c r="K1" s="172" t="s">
         <v>1790</v>
       </c>
-      <c r="K1" s="171"/>
-      <c r="L1" s="171"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L1" s="172"/>
+      <c r="M1" s="172"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>1791</v>
       </c>
@@ -33634,17 +33643,20 @@
       <c r="I2" s="9" t="s">
         <v>1799</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="9" t="s">
+        <v>2623</v>
+      </c>
+      <c r="K2" s="10" t="s">
         <v>1800</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="L2" s="10" t="s">
         <v>1801</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="M2" s="13" t="s">
         <v>1802</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>1803</v>
       </c>
@@ -33672,11 +33684,14 @@
       <c r="I3" s="14" t="s">
         <v>1805</v>
       </c>
-      <c r="J3" s="15"/>
+      <c r="J3" s="14" t="s">
+        <v>1805</v>
+      </c>
       <c r="K3" s="15"/>
-      <c r="L3" s="16"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L3" s="15"/>
+      <c r="M3" s="16"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>1809</v>
       </c>
@@ -33704,15 +33719,18 @@
       <c r="I4" s="14" t="s">
         <v>1811</v>
       </c>
-      <c r="J4" s="21" t="s">
+      <c r="J4" s="14" t="s">
+        <v>2624</v>
+      </c>
+      <c r="K4" s="21" t="s">
         <v>1812</v>
       </c>
-      <c r="K4" s="21" t="s">
+      <c r="L4" s="21" t="s">
         <v>1813</v>
       </c>
-      <c r="L4" s="16"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M4" s="16"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>1814</v>
       </c>
@@ -33740,15 +33758,18 @@
       <c r="I5" s="14" t="s">
         <v>1818</v>
       </c>
-      <c r="J5" s="21" t="s">
+      <c r="J5" s="14" t="s">
+        <v>2625</v>
+      </c>
+      <c r="K5" s="21" t="s">
         <v>1812</v>
       </c>
-      <c r="K5" s="21" t="s">
+      <c r="L5" s="21" t="s">
         <v>1819</v>
       </c>
-      <c r="L5" s="16"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M5" s="16"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>1820</v>
       </c>
@@ -33776,15 +33797,18 @@
       <c r="I6" s="14" t="s">
         <v>1824</v>
       </c>
-      <c r="J6" s="21" t="s">
+      <c r="J6" s="14" t="s">
+        <v>2625</v>
+      </c>
+      <c r="K6" s="21" t="s">
         <v>1812</v>
       </c>
-      <c r="K6" s="21" t="s">
+      <c r="L6" s="21" t="s">
         <v>1819</v>
       </c>
-      <c r="L6" s="16"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M6" s="16"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>1825</v>
       </c>
@@ -33812,15 +33836,18 @@
       <c r="I7" s="14" t="s">
         <v>1828</v>
       </c>
-      <c r="J7" s="21" t="s">
+      <c r="J7" s="14" t="s">
+        <v>2625</v>
+      </c>
+      <c r="K7" s="21" t="s">
         <v>1812</v>
       </c>
-      <c r="K7" s="21" t="s">
+      <c r="L7" s="21" t="s">
         <v>1819</v>
       </c>
-      <c r="L7" s="16"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M7" s="16"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>1829</v>
       </c>
@@ -33848,15 +33875,18 @@
       <c r="I8" s="14" t="s">
         <v>1833</v>
       </c>
-      <c r="J8" s="21" t="s">
+      <c r="J8" s="14" t="s">
+        <v>2625</v>
+      </c>
+      <c r="K8" s="21" t="s">
         <v>1812</v>
       </c>
-      <c r="K8" s="21" t="s">
+      <c r="L8" s="21" t="s">
         <v>1833</v>
       </c>
-      <c r="L8" s="16"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M8" s="16"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>1834</v>
       </c>
@@ -33884,15 +33914,18 @@
       <c r="I9" s="14" t="s">
         <v>1838</v>
       </c>
-      <c r="J9" s="21" t="s">
+      <c r="J9" s="14" t="s">
+        <v>2625</v>
+      </c>
+      <c r="K9" s="21" t="s">
         <v>1812</v>
       </c>
-      <c r="K9" s="21" t="s">
+      <c r="L9" s="21" t="s">
         <v>1839</v>
       </c>
-      <c r="L9" s="16"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M9" s="16"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>1840</v>
       </c>
@@ -33920,15 +33953,18 @@
       <c r="I10" s="14" t="s">
         <v>1844</v>
       </c>
-      <c r="J10" s="21" t="s">
+      <c r="J10" s="14" t="s">
+        <v>2625</v>
+      </c>
+      <c r="K10" s="21" t="s">
         <v>1812</v>
       </c>
-      <c r="K10" s="15" t="s">
+      <c r="L10" s="15" t="s">
         <v>1845</v>
       </c>
-      <c r="L10" s="16"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M10" s="16"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>1846</v>
       </c>
@@ -33956,15 +33992,18 @@
       <c r="I11" s="14" t="s">
         <v>1849</v>
       </c>
-      <c r="J11" s="21" t="s">
+      <c r="J11" s="14" t="s">
+        <v>2625</v>
+      </c>
+      <c r="K11" s="21" t="s">
         <v>1850</v>
       </c>
-      <c r="K11" s="15" t="s">
+      <c r="L11" s="15" t="s">
         <v>1845</v>
       </c>
-      <c r="L11" s="16"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M11" s="16"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>1851</v>
       </c>
@@ -33992,15 +34031,18 @@
       <c r="I12" s="14" t="s">
         <v>1854</v>
       </c>
-      <c r="J12" s="21" t="s">
+      <c r="J12" s="14" t="s">
+        <v>2625</v>
+      </c>
+      <c r="K12" s="21" t="s">
         <v>1850</v>
       </c>
-      <c r="K12" s="15" t="s">
+      <c r="L12" s="15" t="s">
         <v>1845</v>
       </c>
-      <c r="L12" s="16"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M12" s="16"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
         <v>1855</v>
       </c>
@@ -34028,15 +34070,18 @@
       <c r="I13" s="14" t="s">
         <v>1859</v>
       </c>
-      <c r="J13" s="21" t="s">
+      <c r="J13" s="14" t="s">
+        <v>2625</v>
+      </c>
+      <c r="K13" s="21" t="s">
         <v>1850</v>
       </c>
-      <c r="K13" s="15" t="s">
+      <c r="L13" s="15" t="s">
         <v>1845</v>
       </c>
-      <c r="L13" s="16"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M13" s="16"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>1860</v>
       </c>
@@ -34064,15 +34109,18 @@
       <c r="I14" s="14" t="s">
         <v>1863</v>
       </c>
-      <c r="J14" s="21" t="s">
+      <c r="J14" s="14" t="s">
+        <v>2625</v>
+      </c>
+      <c r="K14" s="21" t="s">
         <v>1850</v>
       </c>
-      <c r="K14" s="15" t="s">
+      <c r="L14" s="15" t="s">
         <v>1845</v>
       </c>
-      <c r="L14" s="16"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M14" s="16"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>1864</v>
       </c>
@@ -34100,15 +34148,18 @@
       <c r="I15" s="14" t="s">
         <v>1867</v>
       </c>
-      <c r="J15" s="21" t="s">
+      <c r="J15" s="14" t="s">
+        <v>2625</v>
+      </c>
+      <c r="K15" s="21" t="s">
         <v>1850</v>
       </c>
-      <c r="K15" s="21" t="s">
+      <c r="L15" s="21" t="s">
         <v>1868</v>
       </c>
-      <c r="L15" s="16"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M15" s="16"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>1869</v>
       </c>
@@ -34136,15 +34187,18 @@
       <c r="I16" s="14" t="s">
         <v>1872</v>
       </c>
-      <c r="J16" s="21" t="s">
+      <c r="J16" s="14" t="s">
+        <v>2625</v>
+      </c>
+      <c r="K16" s="21" t="s">
         <v>1850</v>
       </c>
-      <c r="K16" s="21" t="s">
+      <c r="L16" s="21" t="s">
         <v>1868</v>
       </c>
-      <c r="L16" s="16"/>
-    </row>
-    <row r="17" spans="1:12" ht="132.6" x14ac:dyDescent="0.3">
+      <c r="M16" s="16"/>
+    </row>
+    <row r="17" spans="1:13" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="14"/>
       <c r="C17" s="17"/>
@@ -34156,13 +34210,16 @@
         <v>1873</v>
       </c>
       <c r="I17" s="14"/>
-      <c r="J17" s="21"/>
+      <c r="J17" s="14" t="s">
+        <v>2625</v>
+      </c>
       <c r="K17" s="21"/>
-      <c r="L17" s="16" t="s">
+      <c r="L17" s="21"/>
+      <c r="M17" s="16" t="s">
         <v>1874</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
         <v>1703</v>
       </c>
@@ -34190,11 +34247,14 @@
       <c r="I18" s="14" t="s">
         <v>1706</v>
       </c>
-      <c r="J18" s="15"/>
+      <c r="J18" s="14" t="s">
+        <v>2624</v>
+      </c>
       <c r="K18" s="15"/>
-      <c r="L18" s="16"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L18" s="15"/>
+      <c r="M18" s="16"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
         <v>1707</v>
       </c>
@@ -34222,15 +34282,18 @@
       <c r="I19" s="14" t="s">
         <v>1710</v>
       </c>
-      <c r="J19" s="21" t="s">
+      <c r="J19" s="14" t="s">
+        <v>2625</v>
+      </c>
+      <c r="K19" s="21" t="s">
         <v>1812</v>
       </c>
-      <c r="K19" s="21" t="s">
+      <c r="L19" s="21" t="s">
         <v>1711</v>
       </c>
-      <c r="L19" s="16"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M19" s="16"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="14" t="s">
         <v>1712</v>
       </c>
@@ -34258,15 +34321,18 @@
       <c r="I20" s="14" t="s">
         <v>1715</v>
       </c>
-      <c r="J20" s="21" t="s">
+      <c r="J20" s="14" t="s">
+        <v>2625</v>
+      </c>
+      <c r="K20" s="21" t="s">
         <v>1812</v>
       </c>
-      <c r="K20" s="21" t="s">
+      <c r="L20" s="21" t="s">
         <v>1711</v>
       </c>
-      <c r="L20" s="16"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M20" s="16"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
         <v>1716</v>
       </c>
@@ -34294,15 +34360,18 @@
       <c r="I21" s="14" t="s">
         <v>1719</v>
       </c>
-      <c r="J21" s="21" t="s">
+      <c r="J21" s="14" t="s">
+        <v>2625</v>
+      </c>
+      <c r="K21" s="21" t="s">
         <v>1812</v>
       </c>
-      <c r="K21" s="21" t="s">
+      <c r="L21" s="21" t="s">
         <v>1711</v>
       </c>
-      <c r="L21" s="16"/>
-    </row>
-    <row r="22" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="M21" s="16"/>
+    </row>
+    <row r="22" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="133" t="s">
         <v>1889</v>
       </c>
@@ -34330,11 +34399,14 @@
       <c r="I22" s="2" t="s">
         <v>1907</v>
       </c>
-      <c r="J22" s="15"/>
+      <c r="J22" s="14" t="s">
+        <v>2625</v>
+      </c>
       <c r="K22" s="15"/>
-      <c r="L22" s="16"/>
-    </row>
-    <row r="23" spans="1:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L22" s="15"/>
+      <c r="M22" s="16"/>
+    </row>
+    <row r="23" spans="1:13" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="133" t="s">
         <v>1890</v>
       </c>
@@ -34362,11 +34434,14 @@
       <c r="I23" s="2" t="s">
         <v>1912</v>
       </c>
-      <c r="J23" s="15"/>
+      <c r="J23" s="14" t="s">
+        <v>2625</v>
+      </c>
       <c r="K23" s="15"/>
-      <c r="L23" s="16"/>
-    </row>
-    <row r="24" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="L23" s="15"/>
+      <c r="M23" s="16"/>
+    </row>
+    <row r="24" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="133" t="s">
         <v>1891</v>
       </c>
@@ -34394,11 +34469,14 @@
       <c r="I24" s="2" t="s">
         <v>1909</v>
       </c>
-      <c r="J24" s="21"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="16"/>
-    </row>
-    <row r="25" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J24" s="14" t="s">
+        <v>2625</v>
+      </c>
+      <c r="K24" s="21"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="16"/>
+    </row>
+    <row r="25" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="133" t="s">
         <v>1892</v>
       </c>
@@ -34426,11 +34504,14 @@
       <c r="I25" s="2" t="s">
         <v>1915</v>
       </c>
-      <c r="J25" s="21"/>
+      <c r="J25" s="14" t="s">
+        <v>2625</v>
+      </c>
       <c r="K25" s="21"/>
-      <c r="L25" s="16"/>
-    </row>
-    <row r="26" spans="1:12" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L25" s="21"/>
+      <c r="M25" s="16"/>
+    </row>
+    <row r="26" spans="1:13" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="133" t="s">
         <v>1893</v>
       </c>
@@ -34458,11 +34539,14 @@
       <c r="I26" s="2" t="s">
         <v>1916</v>
       </c>
-      <c r="J26" s="21"/>
+      <c r="J26" s="14" t="s">
+        <v>2625</v>
+      </c>
       <c r="K26" s="21"/>
-      <c r="L26" s="16"/>
-    </row>
-    <row r="27" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="L26" s="21"/>
+      <c r="M26" s="16"/>
+    </row>
+    <row r="27" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="133" t="s">
         <v>1894</v>
       </c>
@@ -34490,11 +34574,14 @@
       <c r="I27" s="2" t="s">
         <v>1919</v>
       </c>
-      <c r="J27" s="21"/>
+      <c r="J27" s="14" t="s">
+        <v>2625</v>
+      </c>
       <c r="K27" s="21"/>
-      <c r="L27" s="16"/>
-    </row>
-    <row r="28" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="L27" s="21"/>
+      <c r="M27" s="16"/>
+    </row>
+    <row r="28" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="133" t="s">
         <v>1895</v>
       </c>
@@ -34522,11 +34609,14 @@
       <c r="I28" s="2" t="s">
         <v>2621</v>
       </c>
-      <c r="J28" s="21"/>
+      <c r="J28" s="14" t="s">
+        <v>2625</v>
+      </c>
       <c r="K28" s="21"/>
-      <c r="L28" s="16"/>
-    </row>
-    <row r="29" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="L28" s="21"/>
+      <c r="M28" s="16"/>
+    </row>
+    <row r="29" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="133" t="s">
         <v>1896</v>
       </c>
@@ -34554,11 +34644,14 @@
       <c r="I29" s="2" t="s">
         <v>1921</v>
       </c>
-      <c r="J29" s="21"/>
+      <c r="J29" s="14" t="s">
+        <v>2625</v>
+      </c>
       <c r="K29" s="21"/>
-      <c r="L29" s="16"/>
-    </row>
-    <row r="30" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="L29" s="21"/>
+      <c r="M29" s="16"/>
+    </row>
+    <row r="30" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="133" t="s">
         <v>1897</v>
       </c>
@@ -34586,11 +34679,14 @@
       <c r="I30" s="2" t="s">
         <v>1923</v>
       </c>
-      <c r="J30" s="21"/>
+      <c r="J30" s="14" t="s">
+        <v>2625</v>
+      </c>
       <c r="K30" s="21"/>
-      <c r="L30" s="16"/>
-    </row>
-    <row r="31" spans="1:12" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="L30" s="21"/>
+      <c r="M30" s="16"/>
+    </row>
+    <row r="31" spans="1:13" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A31" s="133" t="s">
         <v>1898</v>
       </c>
@@ -34618,8 +34714,11 @@
       <c r="I31" s="2" t="s">
         <v>1925</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J31" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="133" t="s">
         <v>1899</v>
       </c>
@@ -34647,8 +34746,11 @@
       <c r="I32" s="2" t="s">
         <v>1927</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J32" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="133" t="s">
         <v>1900</v>
       </c>
@@ -34676,8 +34778,11 @@
       <c r="I33" s="2" t="s">
         <v>1905</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J33" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="133" t="s">
         <v>1901</v>
       </c>
@@ -34705,8 +34810,11 @@
       <c r="I34" s="2" t="s">
         <v>1932</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J34" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="133" t="s">
         <v>1902</v>
       </c>
@@ -34734,8 +34842,11 @@
       <c r="I35" s="2" t="s">
         <v>1934</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J35" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="133" t="s">
         <v>1903</v>
       </c>
@@ -34763,8 +34874,11 @@
       <c r="I36" s="2" t="s">
         <v>1937</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J36" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="133" t="s">
         <v>1940</v>
       </c>
@@ -34792,8 +34906,11 @@
       <c r="I37" s="133" t="s">
         <v>2020</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J37" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="133" t="s">
         <v>1941</v>
       </c>
@@ -34821,8 +34938,11 @@
       <c r="I38" s="133" t="s">
         <v>2021</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J38" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="133" t="s">
         <v>1942</v>
       </c>
@@ -34850,8 +34970,11 @@
       <c r="I39" s="133" t="s">
         <v>2022</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J39" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="133" t="s">
         <v>1943</v>
       </c>
@@ -34879,8 +35002,11 @@
       <c r="I40" s="133" t="s">
         <v>2023</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J40" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="133" t="s">
         <v>1944</v>
       </c>
@@ -34908,8 +35034,11 @@
       <c r="I41" s="133" t="s">
         <v>2024</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J41" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="133" t="s">
         <v>1945</v>
       </c>
@@ -34937,8 +35066,11 @@
       <c r="I42" s="133" t="s">
         <v>2025</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J42" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="133" t="s">
         <v>1946</v>
       </c>
@@ -34966,8 +35098,11 @@
       <c r="I43" s="133" t="s">
         <v>2026</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J43" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="133" t="s">
         <v>1947</v>
       </c>
@@ -34995,8 +35130,11 @@
       <c r="I44" s="133" t="s">
         <v>2027</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J44" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="133" t="s">
         <v>1948</v>
       </c>
@@ -35024,8 +35162,11 @@
       <c r="I45" s="133" t="s">
         <v>2028</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J45" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="133" t="s">
         <v>1949</v>
       </c>
@@ -35053,8 +35194,11 @@
       <c r="I46" s="133" t="s">
         <v>2029</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J46" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="133" t="s">
         <v>1950</v>
       </c>
@@ -35082,8 +35226,11 @@
       <c r="I47" s="133" t="s">
         <v>2030</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J47" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="133" t="s">
         <v>1951</v>
       </c>
@@ -35111,8 +35258,11 @@
       <c r="I48" s="133" t="s">
         <v>2031</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J48" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="133" t="s">
         <v>1952</v>
       </c>
@@ -35140,8 +35290,11 @@
       <c r="I49" s="2" t="s">
         <v>1980</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J49" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A50" s="133" t="s">
         <v>1953</v>
       </c>
@@ -35169,8 +35322,11 @@
       <c r="I50" s="2" t="s">
         <v>1982</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J50" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="133" t="s">
         <v>1983</v>
       </c>
@@ -35198,8 +35354,11 @@
       <c r="I51" s="2" t="s">
         <v>2032</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J51" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="133" t="s">
         <v>1984</v>
       </c>
@@ -35227,8 +35386,11 @@
       <c r="I52" s="2" t="s">
         <v>2033</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J52" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="133" t="s">
         <v>1985</v>
       </c>
@@ -35256,8 +35418,11 @@
       <c r="I53" s="2" t="s">
         <v>2034</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J53" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="133" t="s">
         <v>1986</v>
       </c>
@@ -35285,8 +35450,11 @@
       <c r="I54" s="2" t="s">
         <v>2035</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J54" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="133" t="s">
         <v>1987</v>
       </c>
@@ -35314,8 +35482,11 @@
       <c r="I55" s="2" t="s">
         <v>2036</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J55" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="133" t="s">
         <v>1988</v>
       </c>
@@ -35343,8 +35514,11 @@
       <c r="I56" s="2" t="s">
         <v>2037</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J56" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="133" t="s">
         <v>1989</v>
       </c>
@@ -35372,8 +35546,11 @@
       <c r="I57" s="2" t="s">
         <v>2038</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J57" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="133" t="s">
         <v>1990</v>
       </c>
@@ -35401,8 +35578,11 @@
       <c r="I58" s="2" t="s">
         <v>2039</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J58" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="133" t="s">
         <v>1991</v>
       </c>
@@ -35430,8 +35610,11 @@
       <c r="I59" s="2" t="s">
         <v>2040</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J59" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="133" t="s">
         <v>1992</v>
       </c>
@@ -35459,8 +35642,11 @@
       <c r="I60" s="2" t="s">
         <v>2041</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J60" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="133" t="s">
         <v>1993</v>
       </c>
@@ -35488,8 +35674,11 @@
       <c r="I61" s="2" t="s">
         <v>2042</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J61" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="133" t="s">
         <v>1994</v>
       </c>
@@ -35517,8 +35706,11 @@
       <c r="I62" s="2" t="s">
         <v>2043</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J62" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="159" t="s">
         <v>1995</v>
       </c>
@@ -35546,8 +35738,11 @@
       <c r="I63" s="2" t="s">
         <v>2046</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J63" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A64" s="133" t="s">
         <v>2047</v>
       </c>
@@ -35575,8 +35770,11 @@
       <c r="I64" s="2" t="s">
         <v>2263</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J64" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A65" s="133" t="s">
         <v>2048</v>
       </c>
@@ -35604,8 +35802,11 @@
       <c r="I65" s="2" t="s">
         <v>2264</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J65" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A66" s="133" t="s">
         <v>2049</v>
       </c>
@@ -35633,8 +35834,11 @@
       <c r="I66" s="2" t="s">
         <v>2265</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J66" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A67" s="133" t="s">
         <v>2050</v>
       </c>
@@ -35662,8 +35866,11 @@
       <c r="I67" s="2" t="s">
         <v>2266</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J67" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A68" s="133" t="s">
         <v>2051</v>
       </c>
@@ -35691,8 +35898,11 @@
       <c r="I68" s="2" t="s">
         <v>2267</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J68" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A69" s="133" t="s">
         <v>2052</v>
       </c>
@@ -35720,8 +35930,11 @@
       <c r="I69" s="2" t="s">
         <v>2268</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J69" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A70" s="133" t="s">
         <v>2053</v>
       </c>
@@ -35749,8 +35962,11 @@
       <c r="I70" s="2" t="s">
         <v>2269</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J70" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A71" s="133" t="s">
         <v>2054</v>
       </c>
@@ -35778,8 +35994,11 @@
       <c r="I71" s="2" t="s">
         <v>2270</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J71" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A72" s="133" t="s">
         <v>2055</v>
       </c>
@@ -35807,8 +36026,11 @@
       <c r="I72" s="2" t="s">
         <v>2271</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J72" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A73" s="133" t="s">
         <v>2056</v>
       </c>
@@ -35836,8 +36058,11 @@
       <c r="I73" s="2" t="s">
         <v>2272</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J73" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A74" s="133" t="s">
         <v>2057</v>
       </c>
@@ -35865,8 +36090,11 @@
       <c r="I74" s="2" t="s">
         <v>2273</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J74" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A75" s="133" t="s">
         <v>2058</v>
       </c>
@@ -35894,8 +36122,11 @@
       <c r="I75" s="2" t="s">
         <v>2274</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J75" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" s="133" t="s">
         <v>2059</v>
       </c>
@@ -35923,8 +36154,11 @@
       <c r="I76" s="2" t="s">
         <v>2275</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J76" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A77" s="133" t="s">
         <v>2060</v>
       </c>
@@ -35952,8 +36186,11 @@
       <c r="I77" s="2" t="s">
         <v>2276</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J77" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A78" s="133" t="s">
         <v>2061</v>
       </c>
@@ -35981,8 +36218,11 @@
       <c r="I78" s="2" t="s">
         <v>2277</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J78" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A79" s="133" t="s">
         <v>2062</v>
       </c>
@@ -36010,8 +36250,11 @@
       <c r="I79" s="2" t="s">
         <v>2278</v>
       </c>
-    </row>
-    <row r="80" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J79" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A80" s="133" t="s">
         <v>2063</v>
       </c>
@@ -36039,8 +36282,11 @@
       <c r="I80" s="2" t="s">
         <v>2279</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J80" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A81" s="133" t="s">
         <v>2064</v>
       </c>
@@ -36068,8 +36314,11 @@
       <c r="I81" s="2" t="s">
         <v>2280</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J81" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A82" s="133" t="s">
         <v>2065</v>
       </c>
@@ -36097,8 +36346,11 @@
       <c r="I82" s="2" t="s">
         <v>2281</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J82" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A83" s="133" t="s">
         <v>2066</v>
       </c>
@@ -36126,8 +36378,11 @@
       <c r="I83" s="2" t="s">
         <v>2282</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J83" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A84" s="133" t="s">
         <v>2067</v>
       </c>
@@ -36155,8 +36410,11 @@
       <c r="I84" s="2" t="s">
         <v>2283</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J84" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" s="133" t="s">
         <v>2068</v>
       </c>
@@ -36184,8 +36442,11 @@
       <c r="I85" s="2" t="s">
         <v>2284</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J85" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A86" s="133" t="s">
         <v>2069</v>
       </c>
@@ -36213,8 +36474,11 @@
       <c r="I86" s="2" t="s">
         <v>2285</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J86" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" s="133" t="s">
         <v>2070</v>
       </c>
@@ -36242,8 +36506,11 @@
       <c r="I87" s="2" t="s">
         <v>2286</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J87" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A88" s="133" t="s">
         <v>2119</v>
       </c>
@@ -36271,8 +36538,11 @@
       <c r="I88" s="2" t="s">
         <v>2239</v>
       </c>
-    </row>
-    <row r="89" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J88" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A89" s="133" t="s">
         <v>2120</v>
       </c>
@@ -36300,8 +36570,11 @@
       <c r="I89" s="2" t="s">
         <v>2240</v>
       </c>
-    </row>
-    <row r="90" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J89" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A90" s="133" t="s">
         <v>2121</v>
       </c>
@@ -36329,8 +36602,11 @@
       <c r="I90" s="2" t="s">
         <v>2241</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J90" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A91" s="133" t="s">
         <v>2122</v>
       </c>
@@ -36358,8 +36634,11 @@
       <c r="I91" s="2" t="s">
         <v>2242</v>
       </c>
-    </row>
-    <row r="92" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J91" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A92" s="133" t="s">
         <v>2123</v>
       </c>
@@ -36387,8 +36666,11 @@
       <c r="I92" s="2" t="s">
         <v>2243</v>
       </c>
-    </row>
-    <row r="93" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J92" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A93" s="133" t="s">
         <v>2124</v>
       </c>
@@ -36416,8 +36698,11 @@
       <c r="I93" s="2" t="s">
         <v>2244</v>
       </c>
-    </row>
-    <row r="94" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J93" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A94" s="133" t="s">
         <v>2125</v>
       </c>
@@ -36445,8 +36730,11 @@
       <c r="I94" s="2" t="s">
         <v>2245</v>
       </c>
-    </row>
-    <row r="95" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J94" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A95" s="133" t="s">
         <v>2126</v>
       </c>
@@ -36474,8 +36762,11 @@
       <c r="I95" s="2" t="s">
         <v>2246</v>
       </c>
-    </row>
-    <row r="96" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J95" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A96" s="133" t="s">
         <v>2127</v>
       </c>
@@ -36503,8 +36794,11 @@
       <c r="I96" s="2" t="s">
         <v>2247</v>
       </c>
-    </row>
-    <row r="97" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J96" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A97" s="133" t="s">
         <v>2128</v>
       </c>
@@ -36532,8 +36826,11 @@
       <c r="I97" s="2" t="s">
         <v>2248</v>
       </c>
-    </row>
-    <row r="98" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J97" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A98" s="133" t="s">
         <v>2129</v>
       </c>
@@ -36561,8 +36858,11 @@
       <c r="I98" s="2" t="s">
         <v>2249</v>
       </c>
-    </row>
-    <row r="99" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J98" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A99" s="133" t="s">
         <v>2130</v>
       </c>
@@ -36590,8 +36890,11 @@
       <c r="I99" s="2" t="s">
         <v>2250</v>
       </c>
-    </row>
-    <row r="100" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J99" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A100" s="133" t="s">
         <v>2131</v>
       </c>
@@ -36619,8 +36922,11 @@
       <c r="I100" s="2" t="s">
         <v>2251</v>
       </c>
-    </row>
-    <row r="101" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J100" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A101" s="133" t="s">
         <v>2132</v>
       </c>
@@ -36648,8 +36954,11 @@
       <c r="I101" s="2" t="s">
         <v>2252</v>
       </c>
-    </row>
-    <row r="102" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J101" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A102" s="133" t="s">
         <v>2133</v>
       </c>
@@ -36677,8 +36986,11 @@
       <c r="I102" s="2" t="s">
         <v>2253</v>
       </c>
-    </row>
-    <row r="103" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J102" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A103" s="133" t="s">
         <v>2134</v>
       </c>
@@ -36706,8 +37018,11 @@
       <c r="I103" s="2" t="s">
         <v>2254</v>
       </c>
-    </row>
-    <row r="104" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J103" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A104" s="133" t="s">
         <v>2135</v>
       </c>
@@ -36735,8 +37050,11 @@
       <c r="I104" s="2" t="s">
         <v>2255</v>
       </c>
-    </row>
-    <row r="105" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J104" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A105" s="133" t="s">
         <v>2136</v>
       </c>
@@ -36764,8 +37082,11 @@
       <c r="I105" s="2" t="s">
         <v>2256</v>
       </c>
-    </row>
-    <row r="106" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J105" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A106" s="133" t="s">
         <v>2137</v>
       </c>
@@ -36793,8 +37114,11 @@
       <c r="I106" s="2" t="s">
         <v>2257</v>
       </c>
-    </row>
-    <row r="107" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J106" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A107" s="133" t="s">
         <v>2138</v>
       </c>
@@ -36822,8 +37146,11 @@
       <c r="I107" s="2" t="s">
         <v>2258</v>
       </c>
-    </row>
-    <row r="108" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J107" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A108" s="133" t="s">
         <v>2139</v>
       </c>
@@ -36851,8 +37178,11 @@
       <c r="I108" s="2" t="s">
         <v>2259</v>
       </c>
-    </row>
-    <row r="109" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J108" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A109" s="133" t="s">
         <v>2140</v>
       </c>
@@ -36880,8 +37210,11 @@
       <c r="I109" s="2" t="s">
         <v>2260</v>
       </c>
-    </row>
-    <row r="110" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J109" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A110" s="133" t="s">
         <v>2141</v>
       </c>
@@ -36909,8 +37242,11 @@
       <c r="I110" s="2" t="s">
         <v>2261</v>
       </c>
-    </row>
-    <row r="111" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J110" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A111" s="133" t="s">
         <v>2142</v>
       </c>
@@ -36938,8 +37274,11 @@
       <c r="I111" s="2" t="s">
         <v>2262</v>
       </c>
-    </row>
-    <row r="112" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J111" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A112" s="133" t="s">
         <v>2143</v>
       </c>
@@ -36967,8 +37306,11 @@
       <c r="I112" s="2" t="s">
         <v>2227</v>
       </c>
-    </row>
-    <row r="113" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J112" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A113" s="133" t="s">
         <v>2144</v>
       </c>
@@ -36996,8 +37338,11 @@
       <c r="I113" s="2" t="s">
         <v>2228</v>
       </c>
-    </row>
-    <row r="114" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J113" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A114" s="133" t="s">
         <v>2145</v>
       </c>
@@ -37025,8 +37370,11 @@
       <c r="I114" s="2" t="s">
         <v>2229</v>
       </c>
-    </row>
-    <row r="115" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J114" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A115" s="133" t="s">
         <v>2146</v>
       </c>
@@ -37054,8 +37402,11 @@
       <c r="I115" s="2" t="s">
         <v>2230</v>
       </c>
-    </row>
-    <row r="116" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J115" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A116" s="133" t="s">
         <v>2147</v>
       </c>
@@ -37083,8 +37434,11 @@
       <c r="I116" s="2" t="s">
         <v>2231</v>
       </c>
-    </row>
-    <row r="117" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J116" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A117" s="133" t="s">
         <v>2148</v>
       </c>
@@ -37112,8 +37466,11 @@
       <c r="I117" s="2" t="s">
         <v>2232</v>
       </c>
-    </row>
-    <row r="118" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J117" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A118" s="133" t="s">
         <v>2149</v>
       </c>
@@ -37141,8 +37498,11 @@
       <c r="I118" s="2" t="s">
         <v>2233</v>
       </c>
-    </row>
-    <row r="119" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J118" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A119" s="133" t="s">
         <v>2150</v>
       </c>
@@ -37170,8 +37530,11 @@
       <c r="I119" s="2" t="s">
         <v>2234</v>
       </c>
-    </row>
-    <row r="120" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J119" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A120" s="133" t="s">
         <v>2151</v>
       </c>
@@ -37199,8 +37562,11 @@
       <c r="I120" s="2" t="s">
         <v>2235</v>
       </c>
-    </row>
-    <row r="121" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J120" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A121" s="133" t="s">
         <v>2152</v>
       </c>
@@ -37228,8 +37594,11 @@
       <c r="I121" s="2" t="s">
         <v>2236</v>
       </c>
-    </row>
-    <row r="122" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J121" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A122" s="133" t="s">
         <v>2153</v>
       </c>
@@ -37257,8 +37626,11 @@
       <c r="I122" s="2" t="s">
         <v>2237</v>
       </c>
-    </row>
-    <row r="123" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J122" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A123" s="133" t="s">
         <v>2154</v>
       </c>
@@ -37286,8 +37658,11 @@
       <c r="I123" s="2" t="s">
         <v>2238</v>
       </c>
-    </row>
-    <row r="124" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J123" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A124" s="133" t="s">
         <v>2287</v>
       </c>
@@ -37315,8 +37690,11 @@
       <c r="I124" s="2" t="s">
         <v>2290</v>
       </c>
-    </row>
-    <row r="125" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J124" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A125" s="133" t="s">
         <v>2291</v>
       </c>
@@ -37344,8 +37722,11 @@
       <c r="I125" s="2" t="s">
         <v>2294</v>
       </c>
-    </row>
-    <row r="126" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J125" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A126" s="133" t="s">
         <v>2295</v>
       </c>
@@ -37373,8 +37754,11 @@
       <c r="I126" s="2" t="s">
         <v>2298</v>
       </c>
-    </row>
-    <row r="127" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J126" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A127" s="133" t="s">
         <v>2299</v>
       </c>
@@ -37402,8 +37786,11 @@
       <c r="I127" s="2" t="s">
         <v>2302</v>
       </c>
-    </row>
-    <row r="128" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J127" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A128" s="133" t="s">
         <v>2303</v>
       </c>
@@ -37431,8 +37818,11 @@
       <c r="I128" s="2" t="s">
         <v>2306</v>
       </c>
-    </row>
-    <row r="129" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J128" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A129" s="133" t="s">
         <v>2307</v>
       </c>
@@ -37460,8 +37850,11 @@
       <c r="I129" s="2" t="s">
         <v>2310</v>
       </c>
-    </row>
-    <row r="130" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J129" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A130" s="133" t="s">
         <v>2311</v>
       </c>
@@ -37489,8 +37882,11 @@
       <c r="I130" s="2" t="s">
         <v>2314</v>
       </c>
-    </row>
-    <row r="131" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J130" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A131" s="133" t="s">
         <v>2315</v>
       </c>
@@ -37518,8 +37914,11 @@
       <c r="I131" s="2" t="s">
         <v>2318</v>
       </c>
-    </row>
-    <row r="132" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J131" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A132" s="133" t="s">
         <v>2319</v>
       </c>
@@ -37547,8 +37946,11 @@
       <c r="I132" s="2" t="s">
         <v>2322</v>
       </c>
-    </row>
-    <row r="133" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J132" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A133" s="133" t="s">
         <v>2323</v>
       </c>
@@ -37576,8 +37978,11 @@
       <c r="I133" s="2" t="s">
         <v>2326</v>
       </c>
-    </row>
-    <row r="134" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J133" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A134" s="133" t="s">
         <v>2327</v>
       </c>
@@ -37605,8 +38010,11 @@
       <c r="I134" s="2" t="s">
         <v>2330</v>
       </c>
-    </row>
-    <row r="135" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J134" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A135" s="133" t="s">
         <v>2331</v>
       </c>
@@ -37634,8 +38042,11 @@
       <c r="I135" s="2" t="s">
         <v>2334</v>
       </c>
-    </row>
-    <row r="136" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J135" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A136" s="133" t="s">
         <v>2335</v>
       </c>
@@ -37663,8 +38074,11 @@
       <c r="I136" s="2" t="s">
         <v>2338</v>
       </c>
-    </row>
-    <row r="137" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J136" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A137" s="133" t="s">
         <v>2339</v>
       </c>
@@ -37692,8 +38106,11 @@
       <c r="I137" s="2" t="s">
         <v>2342</v>
       </c>
-    </row>
-    <row r="138" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J137" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A138" s="133" t="s">
         <v>2343</v>
       </c>
@@ -37721,8 +38138,11 @@
       <c r="I138" s="2" t="s">
         <v>2346</v>
       </c>
-    </row>
-    <row r="139" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J138" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A139" s="133" t="s">
         <v>2347</v>
       </c>
@@ -37750,8 +38170,11 @@
       <c r="I139" s="2" t="s">
         <v>2350</v>
       </c>
-    </row>
-    <row r="140" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J139" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A140" s="133" t="s">
         <v>2351</v>
       </c>
@@ -37779,8 +38202,11 @@
       <c r="I140" s="2" t="s">
         <v>2354</v>
       </c>
-    </row>
-    <row r="141" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J140" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A141" s="133" t="s">
         <v>2355</v>
       </c>
@@ -37808,8 +38234,11 @@
       <c r="I141" s="2" t="s">
         <v>2358</v>
       </c>
-    </row>
-    <row r="142" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J141" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A142" s="133" t="s">
         <v>2359</v>
       </c>
@@ -37837,8 +38266,11 @@
       <c r="I142" s="2" t="s">
         <v>2362</v>
       </c>
-    </row>
-    <row r="143" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J142" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A143" s="133" t="s">
         <v>2363</v>
       </c>
@@ -37866,8 +38298,11 @@
       <c r="I143" s="2" t="s">
         <v>2366</v>
       </c>
-    </row>
-    <row r="144" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J143" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A144" s="133" t="s">
         <v>2367</v>
       </c>
@@ -37895,8 +38330,11 @@
       <c r="I144" s="2" t="s">
         <v>2370</v>
       </c>
-    </row>
-    <row r="145" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J144" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A145" s="133" t="s">
         <v>2371</v>
       </c>
@@ -37924,8 +38362,11 @@
       <c r="I145" s="2" t="s">
         <v>2374</v>
       </c>
-    </row>
-    <row r="146" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J145" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A146" s="133" t="s">
         <v>2375</v>
       </c>
@@ -37953,8 +38394,11 @@
       <c r="I146" s="2" t="s">
         <v>2378</v>
       </c>
-    </row>
-    <row r="147" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J146" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A147" s="133" t="s">
         <v>2379</v>
       </c>
@@ -37982,8 +38426,11 @@
       <c r="I147" s="2" t="s">
         <v>2382</v>
       </c>
-    </row>
-    <row r="148" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J147" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A148" s="133" t="s">
         <v>2383</v>
       </c>
@@ -38011,8 +38458,11 @@
       <c r="I148" s="2" t="s">
         <v>2386</v>
       </c>
-    </row>
-    <row r="149" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J148" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A149" s="133" t="s">
         <v>2387</v>
       </c>
@@ -38040,8 +38490,11 @@
       <c r="I149" s="2" t="s">
         <v>2390</v>
       </c>
-    </row>
-    <row r="150" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J149" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A150" s="133" t="s">
         <v>2391</v>
       </c>
@@ -38069,8 +38522,11 @@
       <c r="I150" s="2" t="s">
         <v>2394</v>
       </c>
-    </row>
-    <row r="151" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J150" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A151" s="133" t="s">
         <v>2395</v>
       </c>
@@ -38098,8 +38554,11 @@
       <c r="I151" s="2" t="s">
         <v>2398</v>
       </c>
-    </row>
-    <row r="152" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J151" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A152" s="133" t="s">
         <v>2399</v>
       </c>
@@ -38127,8 +38586,11 @@
       <c r="I152" s="2" t="s">
         <v>2402</v>
       </c>
-    </row>
-    <row r="153" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J152" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A153" s="133" t="s">
         <v>2403</v>
       </c>
@@ -38156,8 +38618,11 @@
       <c r="I153" s="2" t="s">
         <v>2406</v>
       </c>
-    </row>
-    <row r="154" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J153" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A154" s="133" t="s">
         <v>2407</v>
       </c>
@@ -38185,8 +38650,11 @@
       <c r="I154" s="2" t="s">
         <v>2410</v>
       </c>
-    </row>
-    <row r="155" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J154" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A155" s="133" t="s">
         <v>2411</v>
       </c>
@@ -38214,8 +38682,11 @@
       <c r="I155" s="2" t="s">
         <v>2414</v>
       </c>
-    </row>
-    <row r="156" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J155" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A156" s="133" t="s">
         <v>2415</v>
       </c>
@@ -38243,8 +38714,11 @@
       <c r="I156" s="2" t="s">
         <v>2418</v>
       </c>
-    </row>
-    <row r="157" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J156" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A157" s="133" t="s">
         <v>2419</v>
       </c>
@@ -38272,8 +38746,11 @@
       <c r="I157" s="2" t="s">
         <v>2422</v>
       </c>
-    </row>
-    <row r="158" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J157" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A158" s="133" t="s">
         <v>2423</v>
       </c>
@@ -38301,8 +38778,11 @@
       <c r="I158" s="2" t="s">
         <v>2426</v>
       </c>
-    </row>
-    <row r="159" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J158" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A159" s="133" t="s">
         <v>2427</v>
       </c>
@@ -38330,8 +38810,11 @@
       <c r="I159" s="2" t="s">
         <v>2430</v>
       </c>
-    </row>
-    <row r="160" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J159" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A160" s="133" t="s">
         <v>2431</v>
       </c>
@@ -38359,8 +38842,11 @@
       <c r="I160" s="2" t="s">
         <v>2434</v>
       </c>
-    </row>
-    <row r="161" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J160" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A161" s="133" t="s">
         <v>2435</v>
       </c>
@@ -38388,8 +38874,11 @@
       <c r="I161" s="2" t="s">
         <v>2438</v>
       </c>
-    </row>
-    <row r="162" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J161" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A162" s="133" t="s">
         <v>2439</v>
       </c>
@@ -38417,8 +38906,11 @@
       <c r="I162" s="2" t="s">
         <v>2442</v>
       </c>
-    </row>
-    <row r="163" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J162" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A163" s="133" t="s">
         <v>2443</v>
       </c>
@@ -38446,8 +38938,11 @@
       <c r="I163" s="2" t="s">
         <v>2446</v>
       </c>
-    </row>
-    <row r="164" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J163" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A164" s="133" t="s">
         <v>2447</v>
       </c>
@@ -38475,8 +38970,11 @@
       <c r="I164" s="2" t="s">
         <v>2450</v>
       </c>
-    </row>
-    <row r="165" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J164" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A165" s="133" t="s">
         <v>2451</v>
       </c>
@@ -38504,8 +39002,11 @@
       <c r="I165" s="2" t="s">
         <v>2454</v>
       </c>
-    </row>
-    <row r="166" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J165" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A166" s="133" t="s">
         <v>2455</v>
       </c>
@@ -38533,8 +39034,11 @@
       <c r="I166" s="2" t="s">
         <v>2458</v>
       </c>
-    </row>
-    <row r="167" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J166" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A167" s="133" t="s">
         <v>2459</v>
       </c>
@@ -38562,8 +39066,11 @@
       <c r="I167" s="2" t="s">
         <v>2462</v>
       </c>
-    </row>
-    <row r="168" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J167" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A168" s="133" t="s">
         <v>2463</v>
       </c>
@@ -38591,8 +39098,11 @@
       <c r="I168" s="2" t="s">
         <v>2466</v>
       </c>
-    </row>
-    <row r="169" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J168" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A169" s="133" t="s">
         <v>2467</v>
       </c>
@@ -38620,8 +39130,11 @@
       <c r="I169" s="2" t="s">
         <v>2470</v>
       </c>
-    </row>
-    <row r="170" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J169" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A170" s="133" t="s">
         <v>2471</v>
       </c>
@@ -38649,8 +39162,11 @@
       <c r="I170" s="2" t="s">
         <v>2474</v>
       </c>
-    </row>
-    <row r="171" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J170" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A171" s="133" t="s">
         <v>2475</v>
       </c>
@@ -38678,8 +39194,11 @@
       <c r="I171" s="2" t="s">
         <v>2478</v>
       </c>
-    </row>
-    <row r="172" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J171" s="14" t="s">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A172" s="133" t="s">
         <v>2479</v>
       </c>
@@ -38707,8 +39226,11 @@
       <c r="I172" s="2" t="s">
         <v>2482</v>
       </c>
-    </row>
-    <row r="173" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J172" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A173" s="133" t="s">
         <v>2483</v>
       </c>
@@ -38736,8 +39258,11 @@
       <c r="I173" s="2" t="s">
         <v>2486</v>
       </c>
-    </row>
-    <row r="174" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J173" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A174" s="133" t="s">
         <v>2487</v>
       </c>
@@ -38765,8 +39290,11 @@
       <c r="I174" s="2" t="s">
         <v>2490</v>
       </c>
-    </row>
-    <row r="175" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J174" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A175" s="133" t="s">
         <v>2491</v>
       </c>
@@ -38794,8 +39322,11 @@
       <c r="I175" s="2" t="s">
         <v>2494</v>
       </c>
-    </row>
-    <row r="176" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J175" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A176" s="133" t="s">
         <v>2495</v>
       </c>
@@ -38823,8 +39354,11 @@
       <c r="I176" s="2" t="s">
         <v>2498</v>
       </c>
-    </row>
-    <row r="177" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J176" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A177" s="133" t="s">
         <v>2499</v>
       </c>
@@ -38852,8 +39386,11 @@
       <c r="I177" s="2" t="s">
         <v>2502</v>
       </c>
-    </row>
-    <row r="178" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J177" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A178" s="133" t="s">
         <v>2503</v>
       </c>
@@ -38881,8 +39418,11 @@
       <c r="I178" s="2" t="s">
         <v>2506</v>
       </c>
-    </row>
-    <row r="179" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J178" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A179" s="133" t="s">
         <v>2507</v>
       </c>
@@ -38910,8 +39450,11 @@
       <c r="I179" s="2" t="s">
         <v>2510</v>
       </c>
-    </row>
-    <row r="180" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J179" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A180" s="133" t="s">
         <v>2511</v>
       </c>
@@ -38939,8 +39482,11 @@
       <c r="I180" s="2" t="s">
         <v>2514</v>
       </c>
-    </row>
-    <row r="181" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J180" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A181" s="133" t="s">
         <v>2515</v>
       </c>
@@ -38968,8 +39514,11 @@
       <c r="I181" s="2" t="s">
         <v>2518</v>
       </c>
-    </row>
-    <row r="182" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J181" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A182" s="133" t="s">
         <v>2519</v>
       </c>
@@ -38997,8 +39546,11 @@
       <c r="I182" s="2" t="s">
         <v>2522</v>
       </c>
-    </row>
-    <row r="183" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J182" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A183" s="133" t="s">
         <v>2523</v>
       </c>
@@ -39026,8 +39578,11 @@
       <c r="I183" s="2" t="s">
         <v>2526</v>
       </c>
-    </row>
-    <row r="184" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J183" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A184" s="133" t="s">
         <v>2527</v>
       </c>
@@ -39055,8 +39610,11 @@
       <c r="I184" s="2" t="s">
         <v>2530</v>
       </c>
-    </row>
-    <row r="185" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J184" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A185" s="133" t="s">
         <v>2531</v>
       </c>
@@ -39084,8 +39642,11 @@
       <c r="I185" s="2" t="s">
         <v>2534</v>
       </c>
-    </row>
-    <row r="186" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J185" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A186" s="133" t="s">
         <v>2535</v>
       </c>
@@ -39113,8 +39674,11 @@
       <c r="I186" s="2" t="s">
         <v>2538</v>
       </c>
-    </row>
-    <row r="187" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J186" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A187" s="133" t="s">
         <v>2539</v>
       </c>
@@ -39142,8 +39706,11 @@
       <c r="I187" s="2" t="s">
         <v>2542</v>
       </c>
-    </row>
-    <row r="188" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J187" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A188" s="133" t="s">
         <v>2543</v>
       </c>
@@ -39171,8 +39738,11 @@
       <c r="I188" s="2" t="s">
         <v>2546</v>
       </c>
-    </row>
-    <row r="189" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J188" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A189" s="133" t="s">
         <v>2547</v>
       </c>
@@ -39200,8 +39770,11 @@
       <c r="I189" s="2" t="s">
         <v>2550</v>
       </c>
-    </row>
-    <row r="190" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J189" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A190" s="133" t="s">
         <v>2551</v>
       </c>
@@ -39229,8 +39802,11 @@
       <c r="I190" s="2" t="s">
         <v>2554</v>
       </c>
-    </row>
-    <row r="191" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J190" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A191" s="133" t="s">
         <v>2555</v>
       </c>
@@ -39258,8 +39834,11 @@
       <c r="I191" s="2" t="s">
         <v>2558</v>
       </c>
-    </row>
-    <row r="192" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J191" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A192" s="133" t="s">
         <v>2559</v>
       </c>
@@ -39287,8 +39866,11 @@
       <c r="I192" s="2" t="s">
         <v>2562</v>
       </c>
-    </row>
-    <row r="193" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J192" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A193" s="133" t="s">
         <v>2563</v>
       </c>
@@ -39316,8 +39898,11 @@
       <c r="I193" s="2" t="s">
         <v>2566</v>
       </c>
-    </row>
-    <row r="194" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J193" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194" s="133" t="s">
         <v>2567</v>
       </c>
@@ -39345,8 +39930,11 @@
       <c r="I194" s="2" t="s">
         <v>2570</v>
       </c>
-    </row>
-    <row r="195" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="J194" s="14" t="s">
+        <v>2624</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A195" s="133" t="s">
         <v>2571</v>
       </c>
@@ -39373,55 +39961,58 @@
       </c>
       <c r="I195" s="2" t="s">
         <v>2574</v>
+      </c>
+      <c r="J195" s="14" t="s">
+        <v>2624</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="K1:M1"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="G4" r:id="rId1"/>
-    <hyperlink ref="J4" r:id="rId2"/>
-    <hyperlink ref="K4" r:id="rId3" location="Patient.identifier"/>
+    <hyperlink ref="K4" r:id="rId2"/>
+    <hyperlink ref="L4" r:id="rId3" location="Patient.identifier"/>
     <hyperlink ref="G5" r:id="rId4"/>
-    <hyperlink ref="J5" r:id="rId5"/>
-    <hyperlink ref="K5" r:id="rId6" location="Patient.address"/>
+    <hyperlink ref="K5" r:id="rId5"/>
+    <hyperlink ref="L5" r:id="rId6" location="Patient.address"/>
     <hyperlink ref="G6" r:id="rId7"/>
-    <hyperlink ref="J6" r:id="rId8"/>
-    <hyperlink ref="K6" r:id="rId9" location="Patient.address"/>
+    <hyperlink ref="K6" r:id="rId8"/>
+    <hyperlink ref="L6" r:id="rId9" location="Patient.address"/>
     <hyperlink ref="G7" r:id="rId10"/>
-    <hyperlink ref="J7" r:id="rId11"/>
-    <hyperlink ref="K7" r:id="rId12" location="Patient.address"/>
+    <hyperlink ref="K7" r:id="rId11"/>
+    <hyperlink ref="L7" r:id="rId12" location="Patient.address"/>
     <hyperlink ref="G8" r:id="rId13"/>
-    <hyperlink ref="J8" r:id="rId14"/>
-    <hyperlink ref="K8" r:id="rId15" location="Patient.birthDate"/>
+    <hyperlink ref="K8" r:id="rId14"/>
+    <hyperlink ref="L8" r:id="rId15" location="Patient.birthDate"/>
     <hyperlink ref="G9" r:id="rId16"/>
-    <hyperlink ref="J9" r:id="rId17"/>
-    <hyperlink ref="K9" r:id="rId18" location="Patient.gender"/>
+    <hyperlink ref="K9" r:id="rId17"/>
+    <hyperlink ref="L9" r:id="rId18" location="Patient.gender"/>
     <hyperlink ref="G10" r:id="rId19"/>
-    <hyperlink ref="J10" r:id="rId20"/>
+    <hyperlink ref="K10" r:id="rId20"/>
     <hyperlink ref="G11" r:id="rId21"/>
-    <hyperlink ref="J11" r:id="rId22"/>
+    <hyperlink ref="K11" r:id="rId22"/>
     <hyperlink ref="G12" r:id="rId23"/>
-    <hyperlink ref="J12" r:id="rId24"/>
+    <hyperlink ref="K12" r:id="rId24"/>
     <hyperlink ref="G13" r:id="rId25"/>
-    <hyperlink ref="J13" r:id="rId26"/>
+    <hyperlink ref="K13" r:id="rId26"/>
     <hyperlink ref="G14" r:id="rId27"/>
-    <hyperlink ref="J14" r:id="rId28"/>
+    <hyperlink ref="K14" r:id="rId28"/>
     <hyperlink ref="G15" r:id="rId29"/>
-    <hyperlink ref="J15" r:id="rId30"/>
-    <hyperlink ref="K15" r:id="rId31" location="Coverage.status"/>
+    <hyperlink ref="K15" r:id="rId30"/>
+    <hyperlink ref="L15" r:id="rId31" location="Coverage.status"/>
     <hyperlink ref="G16" r:id="rId32"/>
-    <hyperlink ref="J16" r:id="rId33"/>
-    <hyperlink ref="K16" r:id="rId34" location="Coverage.status"/>
-    <hyperlink ref="J19" r:id="rId35"/>
-    <hyperlink ref="K19" r:id="rId36" location="Patient.name"/>
-    <hyperlink ref="J20" r:id="rId37"/>
-    <hyperlink ref="K20" r:id="rId38" location="Patient.name"/>
-    <hyperlink ref="J21" r:id="rId39"/>
-    <hyperlink ref="K21" r:id="rId40" location="Patient.name"/>
+    <hyperlink ref="K16" r:id="rId33"/>
+    <hyperlink ref="L16" r:id="rId34" location="Coverage.status"/>
+    <hyperlink ref="K19" r:id="rId35"/>
+    <hyperlink ref="L19" r:id="rId36" location="Patient.name"/>
+    <hyperlink ref="K20" r:id="rId37"/>
+    <hyperlink ref="L20" r:id="rId38" location="Patient.name"/>
+    <hyperlink ref="K21" r:id="rId39"/>
+    <hyperlink ref="L21" r:id="rId40" location="Patient.name"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup orientation="portrait" r:id="rId41"/>
@@ -39456,22 +40047,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="170" t="s">
+      <c r="A1" s="171" t="s">
         <v>1789</v>
       </c>
-      <c r="B1" s="170"/>
-      <c r="C1" s="170"/>
-      <c r="D1" s="170"/>
-      <c r="E1" s="170"/>
-      <c r="F1" s="170"/>
-      <c r="G1" s="170"/>
-      <c r="H1" s="170"/>
-      <c r="I1" s="170"/>
-      <c r="J1" s="171" t="s">
+      <c r="B1" s="171"/>
+      <c r="C1" s="171"/>
+      <c r="D1" s="171"/>
+      <c r="E1" s="171"/>
+      <c r="F1" s="171"/>
+      <c r="G1" s="171"/>
+      <c r="H1" s="171"/>
+      <c r="I1" s="171"/>
+      <c r="J1" s="172" t="s">
         <v>1790</v>
       </c>
-      <c r="K1" s="171"/>
-      <c r="L1" s="171"/>
+      <c r="K1" s="172"/>
+      <c r="L1" s="172"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
@@ -40108,7 +40699,7 @@
   <sheetPr published="0"/>
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="B7" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -40124,22 +40715,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="170" t="s">
+      <c r="A1" s="171" t="s">
         <v>1789</v>
       </c>
-      <c r="B1" s="170"/>
-      <c r="C1" s="170"/>
-      <c r="D1" s="170"/>
-      <c r="E1" s="170"/>
-      <c r="F1" s="170"/>
-      <c r="G1" s="170"/>
-      <c r="H1" s="170"/>
-      <c r="I1" s="170"/>
-      <c r="J1" s="171" t="s">
+      <c r="B1" s="171"/>
+      <c r="C1" s="171"/>
+      <c r="D1" s="171"/>
+      <c r="E1" s="171"/>
+      <c r="F1" s="171"/>
+      <c r="G1" s="171"/>
+      <c r="H1" s="171"/>
+      <c r="I1" s="171"/>
+      <c r="J1" s="172" t="s">
         <v>1790</v>
       </c>
-      <c r="K1" s="171"/>
-      <c r="L1" s="171"/>
+      <c r="K1" s="172"/>
+      <c r="L1" s="172"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
@@ -42316,14 +42907,14 @@
       <c r="E45" s="33"/>
       <c r="F45" s="14"/>
       <c r="G45" s="14"/>
-      <c r="H45" s="172" t="s">
+      <c r="H45" s="173" t="s">
         <v>1587</v>
       </c>
-      <c r="I45" s="172" t="s">
+      <c r="I45" s="173" t="s">
         <v>1587</v>
       </c>
-      <c r="J45" s="172"/>
-      <c r="K45" s="172"/>
+      <c r="J45" s="173"/>
+      <c r="K45" s="173"/>
       <c r="L45" s="34"/>
       <c r="M45"/>
     </row>
@@ -50327,11 +50918,11 @@
       <c r="E103" s="23"/>
       <c r="F103" s="19"/>
       <c r="G103" s="14"/>
-      <c r="H103" s="173" t="s">
+      <c r="H103" s="174" t="s">
         <v>1225</v>
       </c>
-      <c r="I103" s="173"/>
-      <c r="J103" s="173"/>
+      <c r="I103" s="174"/>
+      <c r="J103" s="174"/>
       <c r="K103" s="54"/>
       <c r="L103" s="55"/>
     </row>
@@ -60233,12 +60824,12 @@
       <c r="E276" s="66"/>
       <c r="F276" s="14"/>
       <c r="G276" s="14"/>
-      <c r="H276" s="172" t="s">
+      <c r="H276" s="173" t="s">
         <v>1225</v>
       </c>
-      <c r="I276" s="172"/>
-      <c r="J276" s="172"/>
-      <c r="K276" s="172"/>
+      <c r="I276" s="173"/>
+      <c r="J276" s="173"/>
+      <c r="K276" s="173"/>
       <c r="L276" s="34"/>
     </row>
     <row r="277" spans="1:12" x14ac:dyDescent="0.3">
@@ -69203,12 +69794,12 @@
       <c r="E236" s="23"/>
       <c r="F236" s="14"/>
       <c r="G236" s="14"/>
-      <c r="H236" s="172" t="s">
+      <c r="H236" s="173" t="s">
         <v>1225</v>
       </c>
-      <c r="I236" s="172"/>
-      <c r="J236" s="172"/>
-      <c r="K236" s="172"/>
+      <c r="I236" s="173"/>
+      <c r="J236" s="173"/>
+      <c r="K236" s="173"/>
       <c r="L236" s="34"/>
     </row>
     <row r="237" spans="1:12" x14ac:dyDescent="0.3">
@@ -75513,12 +76104,12 @@
       <c r="E133" s="92"/>
       <c r="F133" s="82"/>
       <c r="G133" s="82"/>
-      <c r="H133" s="174" t="s">
+      <c r="H133" s="175" t="s">
         <v>1225</v>
       </c>
-      <c r="I133" s="174"/>
-      <c r="J133" s="174"/>
-      <c r="K133" s="174"/>
+      <c r="I133" s="175"/>
+      <c r="J133" s="175"/>
+      <c r="K133" s="175"/>
       <c r="L133" s="93"/>
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>